<commit_message>
Updated as on 16Feb
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Finance Laptop\Documents\UiPath\DO and Invoice Process Automation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49FE8EF9-FA8E-4A94-ADDE-B20BACA52A9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A85FC1-CF83-48D3-82F7-F864559CD7C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -223,45 +223,30 @@
     <t>ReportBodyDaily</t>
   </si>
   <si>
-    <t xml:space="preserve">Daily: Final Report for DO and Invoice Process Automation bot for </t>
-  </si>
-  <si>
     <t>ReportSubjectConsolidated</t>
   </si>
   <si>
     <t>ReportBodyConsolidated</t>
   </si>
   <si>
-    <t xml:space="preserve">Consolidated: Final Report for DO and Invoice Process Automation bot for </t>
-  </si>
-  <si>
     <t>ReportSubjectMonthly</t>
   </si>
   <si>
     <t>ReportBodyMonthly</t>
   </si>
   <si>
-    <t xml:space="preserve">Monthly: Final Report for DO and Invoice Process Automation bot for </t>
-  </si>
-  <si>
     <t>ExceptionSubject</t>
   </si>
   <si>
     <t>ExceptionBody</t>
   </si>
   <si>
-    <t>Exception: DO and Invoice Process Automation bot 1</t>
-  </si>
-  <si>
     <t>CCEmailList</t>
   </si>
   <si>
     <t>NoDataSubject</t>
   </si>
   <si>
-    <t>Business Exception: No Data for Bot 1 for</t>
-  </si>
-  <si>
     <t>NoDataBodyDaily</t>
   </si>
   <si>
@@ -272,9 +257,6 @@
   </si>
   <si>
     <t>SDMSPortalLoginBody</t>
-  </si>
-  <si>
-    <t>Error in DO and Invoice Process Automation Bot 1: Failed to Login to SDMS web portal</t>
   </si>
   <si>
     <t>Hello Receiver, 
@@ -425,6 +407,24 @@
 Note: This is auto generated email by bot please don't reply to this.
 Thanks,
 Bot</t>
+  </si>
+  <si>
+    <t>Exception: DO and Invoice Process Automation bot 1  @TodaysDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monthly: Final Report for DO and Invoice Process Automation bot 1 for </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consolidated: Final Report for DO and Invoice Process Automation bot 1 for </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily: Final Report for DO and Invoice Process Automation bot 1 for </t>
+  </si>
+  <si>
+    <t>Business Exception: No Data for Bot 1 for @ProcessType for @TodaysDate</t>
+  </si>
+  <si>
+    <t>Error in DO and Invoice Process Automation Bot 1: Failed to Login to SDMS web portal @TodaysDate</t>
   </si>
 </sst>
 </file>
@@ -815,16 +815,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.5703125" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -862,7 +862,7 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="3" spans="1:26" ht="30">
+    <row r="3" spans="1:26" ht="28.8">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -907,7 +907,7 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
         <v>43</v>
@@ -923,10 +923,10 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B10" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -963,10 +963,10 @@
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B15" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
@@ -998,7 +998,7 @@
         <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="42.6" customHeight="1">
@@ -1006,148 +1006,148 @@
         <v>65</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="25.15" customHeight="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="25.2" customHeight="1">
       <c r="A21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="18.600000000000001" customHeight="1">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15" customHeight="1">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B27" t="s">
-        <v>78</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>83</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1">
       <c r="A33" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B33" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B34" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1">
       <c r="A36" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B36" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B38">
         <v>5</v>
@@ -1155,7 +1155,7 @@
     </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B39">
         <v>10</v>
@@ -1163,7 +1163,7 @@
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B40">
         <v>30</v>
@@ -1171,15 +1171,15 @@
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1">
       <c r="A41" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="14.25" customHeight="1">
       <c r="A42" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B42">
         <v>3</v>
@@ -1187,38 +1187,36 @@
     </row>
     <row r="43" spans="1:2" ht="14.25" customHeight="1">
       <c r="A43" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B43" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="14.25" customHeight="1">
       <c r="A44" t="s">
-        <v>111</v>
-      </c>
-      <c r="B44" s="7">
-        <v>44896</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="B44" s="7"/>
     </row>
     <row r="45" spans="1:2" ht="14.25" customHeight="1">
       <c r="A45" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="14.25" customHeight="1">
       <c r="A46" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="14.25" customHeight="1">
       <c r="A47" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="14.25" customHeight="1">
       <c r="A48" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" ht="14.25" customHeight="1"/>
@@ -2181,12 +2179,12 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.5703125" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2223,7 +2221,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2234,7 +2232,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -2348,7 +2346,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -3345,12 +3343,12 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.42578125" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.44140625" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>